<commit_message>
BWL OP und BMC
</commit_message>
<xml_diff>
--- a/brillianideas/brillianIDEAS/quiz/quiz-questions-template (1).xlsx
+++ b/brillianideas/brillianIDEAS/quiz/quiz-questions-template (1).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="1671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="1697">
   <si>
     <t>questionType</t>
   </si>
@@ -5040,6 +5040,84 @@
   </si>
   <si>
     <t>Gewichtete durchschnittliche Kapitalkosten</t>
+  </si>
+  <si>
+    <t>BWLÖkonomischesPrinzip</t>
+  </si>
+  <si>
+    <t>Das Minimalprinzip beschreibt den Vorgang, ein festgelegtes Ziel mit möglichst wenig Einsatz zu erreichen.</t>
+  </si>
+  <si>
+    <t>Beim Minimalprinzip ist der Input vorgegeben und der Output die zu suchende Größe.</t>
+  </si>
+  <si>
+    <t>Das Maximalprinzip beschreibt den Vorgang, mit festgelegtem Einsatz ein möglichst gutes Ziel zu erreichen.</t>
+  </si>
+  <si>
+    <t>Beim Maximalprinzip ist der Output vorgegeben und der Input die zu suchende Größe.</t>
+  </si>
+  <si>
+    <t>Um wirtschaftlich optimal zu handeln, sollten Einsatz und Ergebnis im optimalen Verhältnis zueinander stehen.</t>
+  </si>
+  <si>
+    <t>Für die Montage eines Autos (Output) sollen möglichst wenige Arbeitsstunden (Aufwand) anfallen.</t>
+  </si>
+  <si>
+    <t>Mit einem Hektar Ackerfläche soll ein möglichst hoher Output erzeugt werden.</t>
+  </si>
+  <si>
+    <t>Der geplante Umsatz eines Unternehmens in Höhe von zehn Millionen Euro soll mit möglichst wenigen Vertriebsmitarbeitern erzielt werden.</t>
+  </si>
+  <si>
+    <t>Ein Autofahrer hat eine definierte Menge an Benzin (Input) und versucht nun mit dieser Menge die größtmögliche Distanz zu fahren (Output).</t>
+  </si>
+  <si>
+    <t>Die Abschlussnote 2,5 soll mit möglichst wenig Lernaufwand erreicht werden.</t>
+  </si>
+  <si>
+    <t>Minimalprinzip</t>
+  </si>
+  <si>
+    <t>Maximalprinzip</t>
+  </si>
+  <si>
+    <t>Eine Nagelfeile wird verwendet, um einen Baum zu fällen.</t>
+  </si>
+  <si>
+    <t>Bei der Reise von Mannheim nach München wird ein direkter ICE gebucht.</t>
+  </si>
+  <si>
+    <t>Im Rahmen einer Kundenzufriedenheitsbefragung geht ein Mitarbeiter von Haus zu Haus und ermittelt die Zufriedenheit einzeln.</t>
+  </si>
+  <si>
+    <t>Um ein kleines Feuer zu löschen werden zwei Liter Champagner verwendet.</t>
+  </si>
+  <si>
+    <t>Ein Fahrrad wird nur mit einem Lappen und Wasser geputzt.</t>
+  </si>
+  <si>
+    <t>Effektivität</t>
+  </si>
+  <si>
+    <t>Effizienz</t>
+  </si>
+  <si>
+    <t>BWLBusinessModelCanvas</t>
+  </si>
+  <si>
+    <t>Die Produktion gehört zu den Key Activities eines Unternehmens.</t>
+  </si>
+  <si>
+    <t>Das Design eines Produktes zählt nicht zur Value Proposition.</t>
+  </si>
+  <si>
+    <t>Der Begriff Customer Segments bezeichnet die Einteilung des Markts in verschiedene Kundengruppen.</t>
+  </si>
+  <si>
+    <t>Der Lieferant ist ein Schlüsselpartner eines Unternehmens.</t>
+  </si>
+  <si>
+    <t>Ein Retailer ist ein Beispiel für einen Vertriebskanal.</t>
   </si>
 </sst>
 </file>
@@ -5490,10 +5568,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet 1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:BD314"/>
+  <dimension ref="A1:BD334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="AJ251" sqref="AJ251"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="O334" sqref="O334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18979,6 +19057,466 @@
       <c r="BC314" s="4"/>
       <c r="BD314" s="4"/>
     </row>
+    <row r="315" spans="1:56" ht="32" x14ac:dyDescent="0.2">
+      <c r="A315" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B315" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C315" s="10" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D315" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E315" t="s">
+        <v>273</v>
+      </c>
+      <c r="O315">
+        <v>1</v>
+      </c>
+      <c r="P315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A316" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C316" s="10" t="s">
+        <v>1673</v>
+      </c>
+      <c r="D316" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E316" t="s">
+        <v>273</v>
+      </c>
+      <c r="O316">
+        <v>0</v>
+      </c>
+      <c r="P316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:56" ht="32" x14ac:dyDescent="0.2">
+      <c r="A317" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B317" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C317" s="10" t="s">
+        <v>1674</v>
+      </c>
+      <c r="D317" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E317" t="s">
+        <v>273</v>
+      </c>
+      <c r="O317">
+        <v>1</v>
+      </c>
+      <c r="P317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A318" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B318" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C318" s="10" t="s">
+        <v>1675</v>
+      </c>
+      <c r="D318" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E318" t="s">
+        <v>273</v>
+      </c>
+      <c r="O318">
+        <v>0</v>
+      </c>
+      <c r="P318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:56" ht="32" x14ac:dyDescent="0.2">
+      <c r="A319" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B319" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C319" s="10" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D319" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E319" t="s">
+        <v>273</v>
+      </c>
+      <c r="O319">
+        <v>1</v>
+      </c>
+      <c r="P319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:56" ht="32" x14ac:dyDescent="0.2">
+      <c r="A320" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C320" s="10" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D320" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E320" t="s">
+        <v>1683</v>
+      </c>
+      <c r="O320">
+        <v>1</v>
+      </c>
+      <c r="P320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A321" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B321" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C321" s="10" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D321" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E321" t="s">
+        <v>1683</v>
+      </c>
+      <c r="O321">
+        <v>0</v>
+      </c>
+      <c r="P321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A322" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B322" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C322" s="10" t="s">
+        <v>1679</v>
+      </c>
+      <c r="D322" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E322" t="s">
+        <v>1683</v>
+      </c>
+      <c r="O322">
+        <v>1</v>
+      </c>
+      <c r="P322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A323" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B323" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C323" s="10" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D323" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E323" t="s">
+        <v>1683</v>
+      </c>
+      <c r="O323">
+        <v>0</v>
+      </c>
+      <c r="P323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A324" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B324" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C324" s="10" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D324" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E324" t="s">
+        <v>1683</v>
+      </c>
+      <c r="O324">
+        <v>1</v>
+      </c>
+      <c r="P324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A325" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B325" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C325" s="10" t="s">
+        <v>1684</v>
+      </c>
+      <c r="D325" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E325" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O325">
+        <v>1</v>
+      </c>
+      <c r="P325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A326" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C326" s="10" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D326" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E326" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O326">
+        <v>0</v>
+      </c>
+      <c r="P326">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A327" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B327" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C327" s="10" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E327" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O327">
+        <v>1</v>
+      </c>
+      <c r="P327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A328" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C328" s="10" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E328" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O328">
+        <v>1</v>
+      </c>
+      <c r="P328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A329" s="5" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B329" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C329" s="10" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E329" t="s">
+        <v>1690</v>
+      </c>
+      <c r="O329">
+        <v>1</v>
+      </c>
+      <c r="P329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A330" s="5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B330" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C330" s="10" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D330" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E330" t="s">
+        <v>273</v>
+      </c>
+      <c r="O330">
+        <v>1</v>
+      </c>
+      <c r="P330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A331" s="5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B331" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C331" s="10" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D331" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E331" t="s">
+        <v>273</v>
+      </c>
+      <c r="O331">
+        <v>1</v>
+      </c>
+      <c r="P331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A332" s="5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B332" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C332" s="10" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D332" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E332" t="s">
+        <v>273</v>
+      </c>
+      <c r="O332">
+        <v>0</v>
+      </c>
+      <c r="P332">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="A333" s="5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B333" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C333" s="10" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D333" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E333" t="s">
+        <v>273</v>
+      </c>
+      <c r="O333">
+        <v>1</v>
+      </c>
+      <c r="P333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A334" s="5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B334" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C334" s="10" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D334" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E334" t="s">
+        <v>273</v>
+      </c>
+      <c r="O334">
+        <v>1</v>
+      </c>
+      <c r="P334">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>